<commit_message>
Adding populations to city changes table
</commit_message>
<xml_diff>
--- a/Data_Clean/Regional_Crime_Rate_Changes_per_100k_2020_2023.xlsx
+++ b/Data_Clean/Regional_Crime_Rate_Changes_per_100k_2020_2023.xlsx
@@ -1,77 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrubval/Desktop/2002_2023_US_Crime_Data/Data_Clean/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E43A6DED-9E36-8A40-9698-CAAAC695809C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="760" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>Murder_Rate_2020_per_100k</t>
-  </si>
-  <si>
-    <t>Murder_Rate_2023_per_100k</t>
-  </si>
-  <si>
-    <t>Change_Murder_Rate_per_100k</t>
-  </si>
-  <si>
-    <t>Violent_Crime_Rate_2020_per_100k</t>
-  </si>
-  <si>
-    <t>Violent_Crime_Rate_2023_per_100k</t>
-  </si>
-  <si>
-    <t>Change_Violent_Crime_Rate_per_100k</t>
-  </si>
-  <si>
-    <t>Property_Crime_Rate_2020_per_100k</t>
-  </si>
-  <si>
-    <t>Property_Crime_Rate_2023_per_100k</t>
-  </si>
-  <si>
-    <t>Change_Property_Crime_Rate_per_100k</t>
-  </si>
-  <si>
-    <t>Midwest</t>
-  </si>
-  <si>
-    <t>National</t>
-  </si>
-  <si>
-    <t>Northeast</t>
-  </si>
-  <si>
-    <t>South</t>
-  </si>
-  <si>
-    <t>West</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,19 +63,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -173,7 +109,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -205,27 +141,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -257,24 +175,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -450,55 +350,70 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="4" max="4" width="31.83203125" customWidth="1"/>
-    <col min="7" max="7" width="29" customWidth="1"/>
-    <col min="10" max="10" width="30.83203125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Region</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Murder_Rate_2020_per_100k</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Murder_Rate_2023_per_100k</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Change_Murder_Rate_per_100k</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Violent_Crime_Rate_2020_per_100k</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Violent_Crime_Rate_2023_per_100k</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Change_Violent_Crime_Rate_per_100k</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Property_Crime_Rate_2020_per_100k</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Property_Crime_Rate_2023_per_100k</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Change_Property_Crime_Rate_per_100k</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>10</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Midwest</t>
+        </is>
       </c>
       <c r="B2">
         <v>7</v>
@@ -507,7 +422,7 @@
         <v>5.5</v>
       </c>
       <c r="D2">
-        <v>-0.214285714285714</v>
+        <v>-0.2142857142857143</v>
       </c>
       <c r="E2">
         <v>387.8</v>
@@ -516,7 +431,7 @@
         <v>338.6</v>
       </c>
       <c r="G2">
-        <v>-0.12686952037132501</v>
+        <v>-0.1268695203713254</v>
       </c>
       <c r="H2">
         <v>1785.5</v>
@@ -525,18 +440,20 @@
         <v>1673</v>
       </c>
       <c r="J2">
-        <v>-6.3007560907308871E-2</v>
+        <v>-0.06300756090730887</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>11</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>National</t>
+        </is>
       </c>
       <c r="B3">
-        <v>6.8318921698087403</v>
+        <v>6.83189216980874</v>
       </c>
       <c r="C3">
-        <v>5.7483260038344968</v>
+        <v>5.748326003834497</v>
       </c>
       <c r="D3">
         <v>-0.158604108355618</v>
@@ -545,10 +462,10 @@
         <v>386.3045018408975</v>
       </c>
       <c r="F3">
-        <v>363.81391756254982</v>
+        <v>363.8139175625498</v>
       </c>
       <c r="G3">
-        <v>-5.821983479656849E-2</v>
+        <v>-0.05821983479656849</v>
       </c>
       <c r="H3">
         <v>1966.869887688033</v>
@@ -557,12 +474,14 @@
         <v>1916.650795719313</v>
       </c>
       <c r="J3">
-        <v>-2.553249316748173E-2</v>
+        <v>-0.02553249316748173</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>12</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Northeast</t>
+        </is>
       </c>
       <c r="B4">
         <v>4.5</v>
@@ -574,13 +493,13 @@
         <v>-0.1777777777777777</v>
       </c>
       <c r="E4">
-        <v>308.39999999999998</v>
+        <v>308.4</v>
       </c>
       <c r="F4">
         <v>289.5</v>
       </c>
       <c r="G4">
-        <v>-6.1284046692606932E-2</v>
+        <v>-0.06128404669260693</v>
       </c>
       <c r="H4">
         <v>1370.6</v>
@@ -589,12 +508,14 @@
         <v>1550.4</v>
       </c>
       <c r="J4">
-        <v>0.13118342331825489</v>
+        <v>0.1311834233182549</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>13</v>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>South</t>
+        </is>
       </c>
       <c r="B5">
         <v>8</v>
@@ -603,7 +524,7 @@
         <v>7.2</v>
       </c>
       <c r="D5">
-        <v>-9.9999999999999978E-2</v>
+        <v>-0.09999999999999998</v>
       </c>
       <c r="E5">
         <v>431.5</v>
@@ -612,7 +533,7 @@
         <v>385.6</v>
       </c>
       <c r="G5">
-        <v>-0.10637311703360371</v>
+        <v>-0.1063731170336037</v>
       </c>
       <c r="H5">
         <v>2106.6</v>
@@ -621,12 +542,14 @@
         <v>1966.1</v>
       </c>
       <c r="J5">
-        <v>-6.6695148580651287E-2</v>
+        <v>-0.06669514858065129</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>14</v>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>West</t>
+        </is>
       </c>
       <c r="B6">
         <v>5.2</v>
@@ -635,7 +558,7 @@
         <v>5</v>
       </c>
       <c r="D6">
-        <v>-3.8461538461538491E-2</v>
+        <v>-0.03846153846153849</v>
       </c>
       <c r="E6">
         <v>418.8</v>
@@ -644,16 +567,16 @@
         <v>448.5</v>
       </c>
       <c r="G6">
-        <v>7.0916905444126044E-2</v>
+        <v>0.07091690544412604</v>
       </c>
       <c r="H6">
         <v>2286.5</v>
       </c>
       <c r="I6">
-        <v>2312.3000000000002</v>
+        <v>2312.3</v>
       </c>
       <c r="J6">
-        <v>1.128362125519361E-2</v>
+        <v>0.01128362125519361</v>
       </c>
     </row>
   </sheetData>

</xml_diff>